<commit_message>
Update Excel file from Streamlit app
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:C308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,23 +5593,6 @@
         </is>
       </c>
     </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>prueba permanente</t>
-        </is>
-      </c>
-      <c r="B309" t="inlineStr">
-        <is>
-          <t>git</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>hub</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: probando by git in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,6 +5593,23 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>probando</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>git</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>hub</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted book: probando from Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:C308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,23 +5593,6 @@
         </is>
       </c>
     </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>probando</t>
-        </is>
-      </c>
-      <c r="B309" t="inlineStr">
-        <is>
-          <t>git</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>hub</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: es de prueba by editorial de prueba in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,6 +5593,23 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>es de prueba</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>editorial de prueba</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>hub</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted book: es de prueba from Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:C308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,23 +5593,6 @@
         </is>
       </c>
     </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>es de prueba</t>
-        </is>
-      </c>
-      <c r="B309" t="inlineStr">
-        <is>
-          <t>editorial de prueba</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>hub</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: prueba by Git in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,6 +5593,23 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Git</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Hub</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deleted book: prueba from Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:C308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,23 +5593,6 @@
         </is>
       </c>
     </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="B309" t="inlineStr">
-        <is>
-          <t>Git</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>Hub</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: Resistencias Letradas by Ana María Ferreira Hernández in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5593,6 +5593,23 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Resistencias Letradas</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Ana María Ferreira Hernández</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Javeriana</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: El peligro de la historia única by Chimamanda Ngozi Adichie in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:C310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5610,6 +5610,23 @@
         </is>
       </c>
     </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>El peligro de la historia única</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Chimamanda Ngozi Adichie</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Random House</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: El quinto hijo by Doris Lessing in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C310"/>
+  <dimension ref="A1:C311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5627,6 +5627,23 @@
         </is>
       </c>
     </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>El quinto hijo</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Doris Lessing</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>DeBolsillo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: La Casa Verde by Mario Vargas Llosa in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C311"/>
+  <dimension ref="A1:C312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5644,6 +5644,23 @@
         </is>
       </c>
     </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>La Casa Verde</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Mario Vargas Llosa</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>DeBolsillo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new book: Muerte en la tarde by Ernest Hemingway in Nini's library
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C312"/>
+  <dimension ref="A1:C313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5661,6 +5661,23 @@
         </is>
       </c>
     </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Muerte en la tarde</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Ernest Hemingway</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>DeBolsillo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added book: prueba to Nini's library from wishlist
</commit_message>
<xml_diff>
--- a/data/Biblioteca_nini.xlsx
+++ b/data/Biblioteca_nini.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C313"/>
+  <dimension ref="A1:C309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5596,87 +5596,15 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Resistencias Letradas</t>
+          <t>prueba</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Ana María Ferreira Hernández</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>Javeriana</t>
-        </is>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="inlineStr">
-        <is>
-          <t>El peligro de la historia única</t>
-        </is>
-      </c>
-      <c r="B310" t="inlineStr">
-        <is>
-          <t>Chimamanda Ngozi Adichie</t>
-        </is>
-      </c>
-      <c r="C310" t="inlineStr">
-        <is>
-          <t>Random House</t>
-        </is>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="inlineStr">
-        <is>
-          <t>El quinto hijo</t>
-        </is>
-      </c>
-      <c r="B311" t="inlineStr">
-        <is>
-          <t>Doris Lessing</t>
-        </is>
-      </c>
-      <c r="C311" t="inlineStr">
-        <is>
-          <t>DeBolsillo</t>
-        </is>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="inlineStr">
-        <is>
-          <t>La Casa Verde</t>
-        </is>
-      </c>
-      <c r="B312" t="inlineStr">
-        <is>
-          <t>Mario Vargas Llosa</t>
-        </is>
-      </c>
-      <c r="C312" t="inlineStr">
-        <is>
-          <t>DeBolsillo</t>
-        </is>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" t="inlineStr">
-        <is>
-          <t>Muerte en la tarde</t>
-        </is>
-      </c>
-      <c r="B313" t="inlineStr">
-        <is>
-          <t>Ernest Hemingway</t>
-        </is>
-      </c>
-      <c r="C313" t="inlineStr">
-        <is>
-          <t>DeBolsillo</t>
-        </is>
-      </c>
+          <t>actualizada</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>